<commit_message>
added work on editing plate readings
</commit_message>
<xml_diff>
--- a/playground/sample_r2_calc.xlsx
+++ b/playground/sample_r2_calc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="13060" yWindow="540" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="13040" yWindow="400" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>fit y</t>
   </si>
@@ -37,6 +37,15 @@
   </si>
   <si>
     <t>r^2</t>
+  </si>
+  <si>
+    <t>t,b</t>
+  </si>
+  <si>
+    <t>t,ec</t>
+  </si>
+  <si>
+    <t>b,ec</t>
   </si>
 </sst>
 </file>
@@ -458,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P32"/>
+  <dimension ref="A1:P30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -976,7 +985,7 @@
         <v>66.965249999999997</v>
       </c>
       <c r="D24">
-        <f t="shared" ref="C24:D24" si="3">AVERAGE(D2:D22)</f>
+        <f t="shared" ref="D24" si="3">AVERAGE(D2:D22)</f>
         <v>49.864336293644001</v>
       </c>
       <c r="F24">
@@ -993,6 +1002,9 @@
       </c>
     </row>
     <row r="28" spans="1:16">
+      <c r="A28" t="s">
+        <v>6</v>
+      </c>
       <c r="B28">
         <v>0.83509999999999995</v>
       </c>
@@ -1005,6 +1017,9 @@
       </c>
     </row>
     <row r="29" spans="1:16">
+      <c r="A29" t="s">
+        <v>7</v>
+      </c>
       <c r="B29">
         <v>-3.1575000000000002</v>
       </c>
@@ -1017,6 +1032,9 @@
       </c>
     </row>
     <row r="30" spans="1:16">
+      <c r="A30" t="s">
+        <v>8</v>
+      </c>
       <c r="B30">
         <v>-2.5958999999999999</v>
       </c>
@@ -1026,25 +1044,6 @@
       <c r="D30">
         <f t="shared" si="4"/>
         <v>1.9470490492024077</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16">
-      <c r="E31" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16">
-      <c r="B32">
-        <f>PRODUCT(B28:B30)</f>
-        <v>6.8449424541750004</v>
-      </c>
-      <c r="D32">
-        <f>PRODUCT(D28:D30)</f>
-        <v>31.242542218904017</v>
-      </c>
-      <c r="E32">
-        <f>(B32/D32) ^ 2</f>
-        <v>4.8000622760763889E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>